<commit_message>
running but poorly, started yolo which runs but crashes VScode
</commit_message>
<xml_diff>
--- a/evaluation_results.xlsx
+++ b/evaluation_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,17 @@
         <v>0.5840266346931458</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>273840.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.6543422341346741</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>